<commit_message>
changed header from address to addressList in customer tab, removed extra rows
</commit_message>
<xml_diff>
--- a/AutomationSeleniumProject/src/main/resources/customer.xlsx
+++ b/AutomationSeleniumProject/src/main/resources/customer.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rneup\IdeaProjects\AutomationTesting-Selenium-Tutorial-0918\AutomationSeleniumProject\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="customer" sheetId="2" r:id="rId5"/>
-    <sheet name="address" sheetId="3" r:id="rId6"/>
-    <sheet name="phone" sheetId="4" r:id="rId7"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="customer" sheetId="2" r:id="rId2"/>
+    <sheet name="address" sheetId="3" r:id="rId3"/>
+    <sheet name="phone" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -194,17 +202,19 @@
   </si>
   <si>
     <t>cellPhone</t>
+  </si>
+  <si>
+    <t>addressList</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="mm/dd/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -221,19 +231,9 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -282,50 +282,33 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,26 +317,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="015E88B1"/>
+      <rgbColor rgb="01EEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -555,7 +597,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -574,7 +616,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +646,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -630,7 +672,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -656,7 +698,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -682,7 +724,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -708,7 +750,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -734,7 +776,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,7 +802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -786,7 +828,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +854,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,9 +867,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -844,7 +892,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -863,7 +911,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,7 +937,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,7 +963,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +989,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -967,7 +1015,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -993,7 +1041,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +1067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1071,7 +1119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,7 +1145,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1110,9 +1158,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1126,7 +1180,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1145,7 +1199,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1255,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1385,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1437,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1396,90 +1450,98 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="3" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="7" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="5">
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" t="s" s="3">
+    <row r="13" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="4"/>
-      <c r="C14" t="s" s="4">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s" s="5">
+      <c r="D14" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1488,192 +1550,178 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'customer'!R1C1" tooltip="" display="customer"/>
-    <hyperlink ref="D12" location="'address'!R1C1" tooltip="" display="address"/>
-    <hyperlink ref="D14" location="'phone'!R1C1" tooltip="" display="phone"/>
+    <hyperlink ref="D10" location="'customer'!R1C1" display="customer"/>
+    <hyperlink ref="D12" location="'address'!R1C1" display="address"/>
+    <hyperlink ref="D14" location="'phone'!R1C1" display="phone"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="6" customWidth="1"/>
-    <col min="2" max="3" width="10.3516" style="6" customWidth="1"/>
-    <col min="4" max="4" width="19.7891" style="6" customWidth="1"/>
-    <col min="5" max="5" width="48.1719" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.85156" style="6" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="5" customWidth="1"/>
+    <col min="2" max="3" width="10.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="48.140625" style="5" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="9">
+      <c r="E1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>36527</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="E2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="9">
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>36924</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="9">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>37317</v>
       </c>
-      <c r="E4" t="s" s="7">
+      <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="9">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="C5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>37713</v>
       </c>
-      <c r="E5" t="s" s="7">
+      <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="9">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>38109</v>
       </c>
-      <c r="E6" t="s" s="7">
+      <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="9">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s" s="7">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>38505</v>
       </c>
-      <c r="E7" t="s" s="7">
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="9">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>38900</v>
       </c>
-      <c r="E8" t="s" s="7">
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1681,200 +1729,200 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.6719" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16" style="11" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="11" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="11" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="11" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="16" style="10" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="10" customWidth="1"/>
+    <col min="7" max="256" width="8.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="D1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s" s="7">
+      <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s" s="7">
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="9">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>12345</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="E2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s" s="7">
+      <c r="F2" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="9">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>54321</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="s" s="7">
+      <c r="F3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="9">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>54322</v>
       </c>
-      <c r="E4" t="s" s="7">
+      <c r="E4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F4" t="s" s="7">
+      <c r="F4" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="9">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>54323</v>
       </c>
-      <c r="E5" t="s" s="7">
+      <c r="E5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F5" t="s" s="7">
+      <c r="F5" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="9">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>54324</v>
       </c>
-      <c r="E6" t="s" s="7">
+      <c r="E6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="s" s="7">
+      <c r="F6" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="9">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s" s="7">
+      <c r="C7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>54325</v>
       </c>
-      <c r="E7" t="s" s="7">
+      <c r="E7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s" s="7">
+      <c r="F7" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="9">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>54326</v>
       </c>
-      <c r="E8" t="s" s="7">
+      <c r="E8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F8" t="s" s="7">
+      <c r="F8" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1882,135 +1930,134 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="12" customWidth="1"/>
-    <col min="2" max="2" width="11.8516" style="12" customWidth="1"/>
-    <col min="3" max="3" width="9.85156" style="12" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="12" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="11" customWidth="1"/>
+    <col min="4" max="256" width="8.85546875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="B1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="9">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>123456</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>1515</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="9">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>123457</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>1516</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="9">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>123458</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>1517</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="9">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>123459</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>1518</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="9">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>123460</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>1519</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="9">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>123461</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>1520</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated data in the Xcel
</commit_message>
<xml_diff>
--- a/AutomationSeleniumProject/src/main/resources/customer.xlsx
+++ b/AutomationSeleniumProject/src/main/resources/customer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -28,10 +28,52 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>customer</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>customer</t>
+    </r>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>address</t>
+    </r>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>phone</t>
+    </r>
   </si>
   <si>
     <t>id</t>
@@ -46,7 +88,7 @@
     <t>dob</t>
   </si>
   <si>
-    <t>address</t>
+    <t>addressList</t>
   </si>
   <si>
     <t>Andy</t>
@@ -121,10 +163,7 @@
     <t>zipCode</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>phone</t>
+    <t>state</t>
   </si>
   <si>
     <t>street address1</t>
@@ -133,7 +172,7 @@
     <t>New York</t>
   </si>
   <si>
-    <t>US</t>
+    <t>NY</t>
   </si>
   <si>
     <t>reference:phone@id#1</t>
@@ -142,13 +181,19 @@
     <t>street address2</t>
   </si>
   <si>
-    <t>New Hamisphere</t>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>NH</t>
   </si>
   <si>
     <t>street address3</t>
   </si>
   <si>
-    <t>North Carolina</t>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>NC</t>
   </si>
   <si>
     <t>reference:phone@id#2</t>
@@ -160,13 +205,19 @@
     <t>Chicago</t>
   </si>
   <si>
+    <t>IL</t>
+  </si>
+  <si>
     <t>reference:phone@id#3</t>
   </si>
   <si>
     <t>street address5</t>
   </si>
   <si>
-    <t>California</t>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>CA</t>
   </si>
   <si>
     <t>reference:phone@id#4</t>
@@ -175,7 +226,10 @@
     <t>street address6</t>
   </si>
   <si>
-    <t>Texas</t>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>TX</t>
   </si>
   <si>
     <t>reference:phone@id#5</t>
@@ -185,6 +239,9 @@
   </si>
   <si>
     <t>Des Moines</t>
+  </si>
+  <si>
+    <t>IA</t>
   </si>
   <si>
     <t>reference:phone@id#6</t>
@@ -237,7 +294,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,8 +313,26 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -267,16 +342,103 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -286,7 +448,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -308,16 +470,70 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -346,7 +562,10 @@
       <rgbColor rgb="015e88b1"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -545,17 +764,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -583,10 +802,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -834,12 +1053,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1126,7 +1345,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1154,10 +1373,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1408,268 +1627,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="256" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="10"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>6</v>
+      </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="10"/>
       <c r="B13" t="s" s="3">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="20"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" ht="13" customHeight="1">
+      <c r="A15" s="7"/>
+      <c r="B15" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" ht="13" customHeight="1">
+      <c r="A16" s="20"/>
+      <c r="B16" s="4"/>
+      <c r="C16" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E16" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'customer'!R1C1" tooltip="" display="customer"/>
-    <hyperlink ref="D12" location="'address'!R1C1" tooltip="" display="address"/>
-    <hyperlink ref="D14" location="'phone'!R1C1" tooltip="" display="phone"/>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
+    <hyperlink ref="D12" location="'customer'!R1C1" tooltip="" display="customer"/>
+    <hyperlink ref="D14" location="'address'!R1C1" tooltip="" display="address"/>
+    <hyperlink ref="D16" location="'phone'!R1C1" tooltip="" display="phone"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="6" customWidth="1"/>
-    <col min="2" max="3" width="10.3516" style="6" customWidth="1"/>
-    <col min="4" max="4" width="19.7891" style="6" customWidth="1"/>
-    <col min="5" max="5" width="48.1719" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.85156" style="6" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="25" customWidth="1"/>
+    <col min="2" max="3" width="10.3516" style="25" customWidth="1"/>
+    <col min="4" max="4" width="19.8516" style="25" customWidth="1"/>
+    <col min="5" max="5" width="48.1719" style="25" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s" s="26">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s" s="26">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s" s="26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="D2" s="28">
+        <v>36527</v>
+      </c>
+      <c r="E2" t="s" s="26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="D3" s="28">
+        <v>36924</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s" s="26">
+        <v>24</v>
+      </c>
+      <c r="D4" s="28">
+        <v>37317</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="26">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s" s="26">
+        <v>27</v>
+      </c>
+      <c r="D5" s="28">
+        <v>37713</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s" s="26">
+        <v>30</v>
+      </c>
+      <c r="D6" s="28">
+        <v>38109</v>
+      </c>
+      <c r="E6" t="s" s="26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="27">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="B7" t="s" s="26">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D7" s="28">
+        <v>38505</v>
+      </c>
+      <c r="E7" t="s" s="26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="27">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="D2" s="10">
-        <v>36527</v>
-      </c>
-      <c r="E2" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="D3" s="10">
-        <v>36924</v>
-      </c>
-      <c r="E3" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="D4" s="10">
-        <v>37317</v>
-      </c>
-      <c r="E4" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="9">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="D5" s="10">
-        <v>37713</v>
-      </c>
-      <c r="E5" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="D6" s="10">
-        <v>38109</v>
-      </c>
-      <c r="E6" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="D7" s="10">
-        <v>38505</v>
-      </c>
-      <c r="E7" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="9">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="B8" t="s" s="26">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s" s="26">
+        <v>36</v>
+      </c>
+      <c r="D8" s="28">
         <v>38900</v>
       </c>
-      <c r="E8" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E8" t="s" s="26">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1682,195 +1971,179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.6719" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16" style="11" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="11" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="11" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="11" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="29" customWidth="1"/>
+    <col min="2" max="2" width="14.6719" style="29" customWidth="1"/>
+    <col min="3" max="3" width="16" style="29" customWidth="1"/>
+    <col min="4" max="5" width="8.85156" style="29" customWidth="1"/>
+    <col min="6" max="6" width="24.5" style="29" customWidth="1"/>
+    <col min="7" max="256" width="8.85156" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s" s="26">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s" s="26">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s" s="26">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="26">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="D2" s="27">
+        <v>12345</v>
+      </c>
+      <c r="E2" t="s" s="26">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s" s="26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s" s="26">
+        <v>47</v>
+      </c>
+      <c r="D3" s="27">
+        <v>54321</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s" s="26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s" s="26">
+        <v>50</v>
+      </c>
+      <c r="D4" s="27">
+        <v>54322</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s" s="26">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="26">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s" s="26">
+        <v>54</v>
+      </c>
+      <c r="D5" s="27">
+        <v>54323</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s" s="26">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="26">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s" s="26">
+        <v>58</v>
+      </c>
+      <c r="D6" s="27">
+        <v>54324</v>
+      </c>
+      <c r="E6" t="s" s="26">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s" s="26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="27">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s" s="7">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="D2" s="9">
-        <v>12345</v>
-      </c>
-      <c r="E2" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s" s="7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="D3" s="9">
-        <v>54321</v>
-      </c>
-      <c r="E3" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s" s="7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="D4" s="9">
-        <v>54322</v>
-      </c>
-      <c r="E4" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s" s="7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="9">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="D5" s="9">
-        <v>54323</v>
-      </c>
-      <c r="E5" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s" s="7">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s" s="7">
-        <v>50</v>
-      </c>
-      <c r="D6" s="9">
-        <v>54324</v>
-      </c>
-      <c r="E6" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s" s="7">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s" s="7">
-        <v>53</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="B7" t="s" s="26">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s" s="26">
+        <v>62</v>
+      </c>
+      <c r="D7" s="27">
         <v>54325</v>
       </c>
-      <c r="E7" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s" s="7">
-        <v>54</v>
+      <c r="E7" t="s" s="26">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s" s="26">
+        <v>64</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="9">
+      <c r="A8" s="27">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="7">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s" s="7">
-        <v>56</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="B8" t="s" s="26">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="D8" s="27">
         <v>54326</v>
       </c>
-      <c r="E8" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s" s="7">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E8" t="s" s="26">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s" s="26">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1883,130 +2156,94 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="12" customWidth="1"/>
-    <col min="2" max="2" width="11.8516" style="12" customWidth="1"/>
-    <col min="3" max="3" width="9.85156" style="12" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="12" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="30" customWidth="1"/>
+    <col min="2" max="2" width="16.6719" style="30" customWidth="1"/>
+    <col min="3" max="3" width="15.8516" style="30" customWidth="1"/>
+    <col min="4" max="256" width="8.85156" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s" s="26">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27">
+        <v>5152229999</v>
+      </c>
+      <c r="C2" s="27">
+        <v>3191237890</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27">
+        <v>5159991111</v>
+      </c>
+      <c r="C3" s="27">
+        <v>3193334444</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27">
+        <v>5153332222</v>
+      </c>
+      <c r="C4" s="27">
+        <v>3191112222</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27">
+        <v>5150003333</v>
+      </c>
+      <c r="C5" s="27">
+        <v>3195552222</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27">
+        <v>5156662222</v>
+      </c>
+      <c r="C6" s="27">
+        <v>3196667777</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="27">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>59</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9">
-        <v>123456</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1515</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9">
-        <v>123457</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1516</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9">
-        <v>123458</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1517</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="9">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9">
-        <v>123459</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1518</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9">
-        <v>123460</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1519</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9">
-        <v>123461</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1520</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B7" s="27">
+        <v>5151118888</v>
+      </c>
+      <c r="C7" s="27">
+        <v>3199992222</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>